<commit_message>
added jmx file and latest run reports
</commit_message>
<xml_diff>
--- a/TC_Manual_Test_Managing_Report_Templates_20240906_Atosh.xlsx
+++ b/TC_Manual_Test_Managing_Report_Templates_20240906_Atosh.xlsx
@@ -8,7 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atosh\ATOSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E88A4E-9C7C-4897-92DB-FD5B0D73EABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5FA5F0-6CFD-4FC4-990A-C699D5B3D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1QCT4bC0PCnn0W2klRE7XTtybpYRmWaEAs6A+Octok6arLyDF3sY3FTA2xKHnS63nVbQ9xDUBJyMOHsHgQxKyg==" workbookSaltValue="6TliIx7O9ZMPR8u7t4pDUg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1025,59 +1026,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1300,7 +1301,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1311,39 +1312,39 @@
     <col min="4" max="4" width="44" style="1" customWidth="1"/>
     <col min="5" max="5" width="39.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.6328125" style="1" customWidth="1"/>
-    <col min="7" max="9" width="12.6328125" style="20"/>
+    <col min="7" max="9" width="12.6328125" style="14"/>
     <col min="10" max="16384" width="12.6328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="20" customFormat="1" ht="19" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="19" customHeight="1">
+      <c r="A1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1366,13 +1367,13 @@
       <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="4"/>
@@ -1396,13 +1397,13 @@
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J3" s="4"/>
@@ -1426,13 +1427,13 @@
       <c r="F4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J4" s="4"/>
@@ -1456,13 +1457,13 @@
       <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J5" s="4"/>
@@ -1486,13 +1487,13 @@
       <c r="F6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="4"/>
@@ -1516,13 +1517,13 @@
       <c r="F7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J7" s="4"/>
@@ -1546,13 +1547,13 @@
       <c r="F8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J8" s="4"/>
@@ -1576,13 +1577,13 @@
       <c r="F9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="G9" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J9" s="4"/>
@@ -1606,13 +1607,13 @@
       <c r="F10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="G10" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J10" s="4"/>
@@ -1636,13 +1637,13 @@
       <c r="F11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J11" s="4"/>
@@ -1666,13 +1667,13 @@
       <c r="F12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J12" s="4"/>
@@ -1696,13 +1697,13 @@
       <c r="F13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="G13" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J13" s="4"/>
@@ -1726,13 +1727,13 @@
       <c r="F14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J14" s="4"/>
@@ -1756,13 +1757,13 @@
       <c r="F15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="13" t="s">
+      <c r="G15" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J15" s="4"/>
@@ -1786,13 +1787,13 @@
       <c r="F16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H16" s="13" t="s">
+      <c r="G16" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J16" s="4"/>
@@ -1816,13 +1817,13 @@
       <c r="F17" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="13" t="s">
+      <c r="G17" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J17" s="4"/>
@@ -1846,13 +1847,13 @@
       <c r="F18" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="G18" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="4"/>
@@ -1876,13 +1877,13 @@
       <c r="F19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="13" t="s">
+      <c r="G19" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J19" s="4"/>
@@ -1906,13 +1907,13 @@
       <c r="F20" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="13" t="s">
+      <c r="G20" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="11" t="s">
         <v>2</v>
       </c>
       <c r="J20" s="4"/>
@@ -1936,18 +1937,19 @@
       <c r="F21" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="13" t="s">
+      <c r="G21" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J21" s="4"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="QMM8jJQdw/zizqbvMLnATxhFr4tZSjWbrl1zIUhE2uTkeuX8pT76dXrqvKZXm5xCpYT8YNbbzwhp3GqZyGCFzg==" saltValue="KMytEQDVb6BGWab8Yz7BRA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H21" xr:uid="{104F241F-8ED9-4C34-A31C-A0D9C12727E2}">
       <formula1>"High,Medium,Low"</formula1>
@@ -1965,7 +1967,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1976,382 +1978,352 @@
     <col min="4" max="4" width="39" style="7" customWidth="1"/>
     <col min="5" max="5" width="22.81640625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="20"/>
+    <col min="7" max="7" width="8.7265625" style="14"/>
     <col min="8" max="9" width="8.7265625" style="2"/>
     <col min="10" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="22" customFormat="1" ht="14.5" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="14.5" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="43" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="10"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="43" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10" ht="43" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="10"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:10" ht="43" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" ht="43" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="10"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10" ht="61" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="43" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10" ht="43" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="10"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" ht="75.5" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" ht="66.5" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="11"/>
+      <c r="G12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="43" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" spans="1:10" ht="61.5" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="10"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Xa4E51uGiJz6nbzMFzbdy5uBBEpfuoKwY3DTz3I+5obkbyxcQ9kl5z5WcptkvsgKea8Pu0U+eGJUKPnZxC3Gyg==" saltValue="qdVJXdiSmXaObV7bdsxfJw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="47">
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
@@ -2368,6 +2340,37 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I4 I6 I8:I9 I11 I13" xr:uid="{3564E509-AC25-40ED-ABCF-CC901B603CDB}">

</xml_diff>